<commit_message>
[ANV] added shielding spreadsheet
</commit_message>
<xml_diff>
--- a/SOURCES/sources_running/data/raw_sources_IO/shielding.xlsx
+++ b/SOURCES/sources_running/data/raw_sources_IO/shielding.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/SOURCES/sources_running/data/raw_sources_IO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65510BA6-B467-0843-BF8C-1817E0ED8A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EC2AF5-3195-864F-981E-9ADC481DA887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Shotcrete Density" sheetId="5" r:id="rId1"/>
     <sheet name="Shotcrete Hang" sheetId="7" r:id="rId2"/>
     <sheet name="Norite" sheetId="9" r:id="rId3"/>
+    <sheet name="Attenuation Coefficients" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
   <si>
     <t>Z (atomic number)</t>
   </si>
@@ -116,6 +117,21 @@
   </si>
   <si>
     <t>difference (%)</t>
+  </si>
+  <si>
+    <t>Shotcrete</t>
+  </si>
+  <si>
+    <t>Isotope (A)</t>
+  </si>
+  <si>
+    <t>Isotope Fraction</t>
+  </si>
+  <si>
+    <t>Microscopic Elastic Cross Section [JENDL 5.0 Fission Spectrum Average] (b)</t>
+  </si>
+  <si>
+    <t>Norite</t>
   </si>
 </sst>
 </file>
@@ -131,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +169,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -184,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -195,6 +223,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,7 +550,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1255,7 +1288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0217FC4-E926-2C49-9B03-6A0A2D04B16C}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+    <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -1723,4 +1756,120 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A233B61-36A1-4C4B-B35C-C40FECD0EA60}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>2.9660000000000002</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>2.7010000000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.96940999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[ANV] added some values to shielding spreadsheet
</commit_message>
<xml_diff>
--- a/SOURCES/sources_running/data/raw_sources_IO/shielding.xlsx
+++ b/SOURCES/sources_running/data/raw_sources_IO/shielding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/SOURCES/sources_running/data/raw_sources_IO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4A5FC7-BA0A-5B4A-87C9-BE96D9A003C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7493C086-7211-454F-A03A-610B120DC294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
@@ -1333,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0217FC4-E926-2C49-9B03-6A0A2D04B16C}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1401,13 +1401,16 @@
         <f>$E$2*(C2/100)</f>
         <v>4.0800000000000003E-2</v>
       </c>
-      <c r="H2" t="e">
+      <c r="G2">
+        <v>1.008</v>
+      </c>
+      <c r="H2">
         <f>(F2/G2)*6.0221408E+23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I2" t="e">
+        <v>2.437533180952381E+22</v>
+      </c>
+      <c r="I2">
         <f>H2/$H$14</f>
-        <v>#DIV/0!</v>
+        <v>3.0944270730150422E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1424,13 +1427,16 @@
         <f t="shared" ref="F3:F13" si="0">$E$2*(C3/100)</f>
         <v>1.0880000000000003E-2</v>
       </c>
-      <c r="H3" t="e">
-        <f t="shared" ref="H3:H12" si="1">(F3/G3)*6.0221408E+23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I3" t="e">
-        <f t="shared" ref="I3:I12" si="2">H3/$H$14</f>
-        <v>#DIV/0!</v>
+      <c r="G3">
+        <v>12.010999999999999</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H13" si="1">(F3/G3)*6.0221408E+23</f>
+        <v>5.4550738409791042E+20</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I13" si="2">H3/$H$14</f>
+        <v>6.9251685723623643E-4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1447,13 +1453,16 @@
         <f t="shared" si="0"/>
         <v>12.512000000000002</v>
       </c>
-      <c r="H4" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I4" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="G4">
+        <v>15.999000000000001</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>4.709608456128509E+23</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0.59788067804888434</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1470,13 +1479,16 @@
         <f t="shared" si="0"/>
         <v>0.59840000000000015</v>
       </c>
-      <c r="H5" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I5" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="G5">
+        <v>22.99</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1.5674854522488044E+22</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>1.9899090842737884E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1493,13 +1505,16 @@
         <f t="shared" si="0"/>
         <v>0.89760000000000018</v>
       </c>
-      <c r="H6" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I6" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="G6">
+        <v>24.305</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>2.2240171084468218E+22</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>2.8233702847636939E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1516,13 +1531,16 @@
         <f t="shared" si="0"/>
         <v>2.448</v>
       </c>
-      <c r="H7" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I7" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="G7">
+        <v>26.981999999999999</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>5.4637168032021349E+22</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>6.9361407373786141E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1539,13 +1557,16 @@
         <f t="shared" si="0"/>
         <v>7.1264000000000012</v>
       </c>
-      <c r="H8" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="G8">
+        <v>28.085000000000001</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1.5280820436930748E+23</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>0.19398868014360707</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1562,13 +1583,16 @@
         <f t="shared" si="0"/>
         <v>0.32640000000000002</v>
       </c>
-      <c r="H9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="G9">
+        <v>39.097999999999999</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>5.0274355647859225E+21</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>6.3822855176206708E-3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1585,13 +1609,16 @@
         <f t="shared" si="0"/>
         <v>1.4144000000000003</v>
       </c>
-      <c r="H10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="G10">
+        <v>40.078000000000003</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>2.1252846817505865E+22</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>2.6980303318388552E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1608,13 +1635,16 @@
         <f t="shared" si="0"/>
         <v>2.7200000000000002E-2</v>
       </c>
-      <c r="H11" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="G11">
+        <v>54.938000000000002</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>2.9815834169427355E+20</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>3.7850940934619178E-4</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1631,13 +1661,16 @@
         <f t="shared" si="0"/>
         <v>1.6864000000000001</v>
       </c>
-      <c r="H12" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I12" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="G12">
+        <v>55.844999999999999</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>1.8185581959208526E+22</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>2.3086437383847924E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1653,6 +1686,17 @@
       <c r="F13">
         <f t="shared" si="0"/>
         <v>0.13600000000000001</v>
+      </c>
+      <c r="G13">
+        <v>47.866999999999997</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>1.7110141617398208E+21</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>2.1721175267575871E-3</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1660,13 +1704,13 @@
         <f>SUM(F2:F13)</f>
         <v>27.22448</v>
       </c>
-      <c r="H14" s="3" t="e">
-        <f>SUM(H2:H12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I14" s="3" t="e">
-        <f>SUM(I2:I12)</f>
-        <v>#DIV/0!</v>
+      <c r="H14" s="3">
+        <f>SUM(H2:H13)</f>
+        <v>7.8771711965969219E+23</v>
+      </c>
+      <c r="I14" s="3">
+        <f>SUM(I2:I13)</f>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1692,7 +1736,7 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <v>8.3693831226593299E-3</v>
+        <v>3.0944270730150422E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1700,7 +1744,7 @@
         <v>6</v>
       </c>
       <c r="B24">
-        <v>7.022728404246925E-4</v>
+        <v>6.9251685723623643E-4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1708,7 +1752,7 @@
         <v>8</v>
       </c>
       <c r="B25">
-        <v>0.63266447300513629</v>
+        <v>0.59788067804888434</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1716,7 +1760,7 @@
         <v>11</v>
       </c>
       <c r="B26">
-        <v>2.063825428636017E-2</v>
+        <v>1.9899090842737884E-2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1724,7 +1768,7 @@
         <v>12</v>
       </c>
       <c r="B27">
-        <v>1.023791290051672E-2</v>
+        <v>2.8233702847636939E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1732,7 +1776,7 @@
         <v>13</v>
       </c>
       <c r="B28">
-        <v>4.720578993057023E-2</v>
+        <v>6.9361407373786141E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1740,7 +1784,7 @@
         <v>14</v>
       </c>
       <c r="B29">
-        <v>0.20948218342998465</v>
+        <v>0.19398868014360707</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1748,7 +1792,7 @@
         <v>19</v>
       </c>
       <c r="B30">
-        <v>9.492483299759916E-3</v>
+        <v>6.3822855176206708E-3</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1756,26 +1800,37 @@
         <v>20</v>
       </c>
       <c r="B31">
-        <v>5.0195800241836508E-2</v>
+        <v>2.6980303318388552E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B32">
-        <v>1.4202133142682343E-3</v>
+        <v>2.1721175267575871E-3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
+        <v>25</v>
+      </c>
+      <c r="B33">
+        <v>3.7850940934619178E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>26</v>
       </c>
-      <c r="B33">
-        <v>9.5912336284833428E-3</v>
+      <c r="B34">
+        <v>2.3086437383847924E-2</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:B34">
+    <sortCondition ref="A23:A34"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
[ANV] updated mean free path stuff
</commit_message>
<xml_diff>
--- a/SOURCES/sources_running/data/raw_sources_IO/shielding.xlsx
+++ b/SOURCES/sources_running/data/raw_sources_IO/shielding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/SOURCES/sources_running/data/raw_sources_IO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7493C086-7211-454F-A03A-610B120DC294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37F8608-F128-1A45-9DB6-B509E358EE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Shotcrete Density" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
   <si>
     <t>Z (atomic number)</t>
   </si>
@@ -1335,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0217FC4-E926-2C49-9B03-6A0A2D04B16C}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1837,10 +1837,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A233B61-36A1-4C4B-B35C-C40FECD0EA60}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2317,6 +2317,435 @@
         <v>34</v>
       </c>
     </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>3.927</v>
+      </c>
+      <c r="D17">
+        <f>C17*1E-24</f>
+        <v>3.9269999999999997E-24</v>
+      </c>
+      <c r="E17">
+        <v>0.99972000000000005</v>
+      </c>
+      <c r="F17">
+        <f>Norite!H2</f>
+        <v>2.437533180952381E+22</v>
+      </c>
+      <c r="G17">
+        <f>F17*E17</f>
+        <v>2.4368506716617146E+22</v>
+      </c>
+      <c r="H17">
+        <f>D17*F17</f>
+        <v>9.5721928015999991E-2</v>
+      </c>
+      <c r="I17">
+        <f>1/H17</f>
+        <v>10.44692705973128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>2.3380000000000001</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:D28" si="4">C18*1E-24</f>
+        <v>2.338E-24</v>
+      </c>
+      <c r="E18">
+        <v>0.98839999999999995</v>
+      </c>
+      <c r="F18">
+        <f>Norite!H3</f>
+        <v>5.4550738409791042E+20</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18:G28" si="5">F18*E18</f>
+        <v>5.3917949844237464E+20</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H28" si="6">D18*F18</f>
+        <v>1.2753962640209145E-3</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ref="I18:I28" si="7">1/H18</f>
+        <v>784.07004019858221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>2.7559999999999998</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="4"/>
+        <v>2.7559999999999995E-24</v>
+      </c>
+      <c r="E19">
+        <v>0.99738000000000004</v>
+      </c>
+      <c r="F19">
+        <f>Norite!H4</f>
+        <v>4.709608456128509E+23</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>4.6972692819734522E+23</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="6"/>
+        <v>1.297968090509017</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="7"/>
+        <v>0.77043496470536155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>2.7</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="4"/>
+        <v>2.7000000000000001E-24</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f>Norite!H5</f>
+        <v>1.5674854522488044E+22</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>1.5674854522488044E+22</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="6"/>
+        <v>4.2322107210717719E-2</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="7"/>
+        <v>23.628313094645684</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>24</v>
+      </c>
+      <c r="C21">
+        <v>3.145</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="4"/>
+        <v>3.1449999999999997E-24</v>
+      </c>
+      <c r="E21">
+        <v>0.78879999999999995</v>
+      </c>
+      <c r="F21">
+        <f>Norite!H6</f>
+        <v>2.2240171084468218E+22</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>1.7543046951428529E+22</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="6"/>
+        <v>6.9945338060652534E-2</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="7"/>
+        <v>14.296878501507249</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>2.9660000000000002</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="4"/>
+        <v>2.9660000000000001E-24</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f>Norite!H7</f>
+        <v>5.4637168032021349E+22</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>5.4637168032021349E+22</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="6"/>
+        <v>0.16205384038297532</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="7"/>
+        <v>6.1707886566386838</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <v>2.99</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="4"/>
+        <v>2.99E-24</v>
+      </c>
+      <c r="E23">
+        <v>0.92191000000000001</v>
+      </c>
+      <c r="F23">
+        <f>Norite!H8</f>
+        <v>1.5280820436930748E+23</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>1.4087541169010827E+23</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="6"/>
+        <v>0.45689653106422934</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="7"/>
+        <v>2.1886793442505312</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>39</v>
+      </c>
+      <c r="C24">
+        <v>2.6539999999999999</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="4"/>
+        <v>2.6539999999999998E-24</v>
+      </c>
+      <c r="E24">
+        <v>0.93258099999999999</v>
+      </c>
+      <c r="F24">
+        <f>Norite!H9</f>
+        <v>5.0274355647859225E+21</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>4.6884908864436201E+21</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="6"/>
+        <v>1.3342813988941837E-2</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="7"/>
+        <v>74.946709204578056</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>2.7010000000000001</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="4"/>
+        <v>2.7009999999999999E-24</v>
+      </c>
+      <c r="E25">
+        <v>0.96940999999999999</v>
+      </c>
+      <c r="F25">
+        <f>Norite!H10</f>
+        <v>2.1252846817505865E+22</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>2.0602722233358362E+22</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="6"/>
+        <v>5.7403939254083339E-2</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="7"/>
+        <v>17.420407257658134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26">
+        <v>55</v>
+      </c>
+      <c r="C26">
+        <v>2.5880000000000001</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="4"/>
+        <v>2.588E-24</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f>Norite!H11</f>
+        <v>2.9815834169427355E+20</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>2.9815834169427355E+20</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="6"/>
+        <v>7.7163378830477994E-4</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="7"/>
+        <v>1295.9515448344</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>56</v>
+      </c>
+      <c r="C27">
+        <v>2.5880000000000001</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="4"/>
+        <v>2.588E-24</v>
+      </c>
+      <c r="E27">
+        <v>0.91754000000000002</v>
+      </c>
+      <c r="F27">
+        <f>Norite!H12</f>
+        <v>1.8185581959208526E+22</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>1.6685998870852192E+22</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="6"/>
+        <v>4.7064286110431668E-2</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="7"/>
+        <v>21.247533589558746</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28">
+        <v>48</v>
+      </c>
+      <c r="C28">
+        <v>2.661</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="4"/>
+        <v>2.661E-24</v>
+      </c>
+      <c r="E28">
+        <v>0.73719999999999997</v>
+      </c>
+      <c r="F28">
+        <f>Norite!H13</f>
+        <v>1.7110141617398208E+21</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>1.2613596400345958E+21</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="6"/>
+        <v>4.5530086843896629E-3</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="7"/>
+        <v>219.63498629567218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="15">
+        <f>SUM(F17:F28)</f>
+        <v>7.8771711965969219E+23</v>
+      </c>
+      <c r="G29" s="15">
+        <f>SUM(G18:G28)</f>
+        <v>7.4253331886421672E+23</v>
+      </c>
+      <c r="H29" s="15">
+        <f>SUM(H18:H28)</f>
+        <v>2.1535969853177641</v>
+      </c>
+      <c r="I29" s="15">
+        <f t="shared" ref="I29" si="8">1/H29</f>
+        <v>0.46433943157310353</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[ANV] updated the shielding spreadsheet
</commit_message>
<xml_diff>
--- a/SOURCES/sources_running/data/raw_sources_IO/shielding.xlsx
+++ b/SOURCES/sources_running/data/raw_sources_IO/shielding.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Research/n-elec-scattering/SOURCES/sources_running/data/raw_sources_IO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B26B13-64B1-7343-AA29-C6549D240FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4D258F-F9EB-8344-80A9-4AE3E61C7DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
+    <workbookView xWindow="920" yWindow="1260" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{37FEC5E8-CE26-3C43-983C-91CF58415182}"/>
   </bookViews>
   <sheets>
     <sheet name="Shotcrete Density" sheetId="5" r:id="rId1"/>
     <sheet name="Shotcrete Hang" sheetId="7" r:id="rId2"/>
-    <sheet name="Norite" sheetId="9" r:id="rId3"/>
+    <sheet name="Norite Density" sheetId="9" r:id="rId3"/>
     <sheet name="Attenuation Coefficients" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -1335,7 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0217FC4-E926-2C49-9B03-6A0A2D04B16C}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -1839,7 +1839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A233B61-36A1-4C4B-B35C-C40FECD0EA60}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -2335,7 +2335,7 @@
         <v>0.99972000000000005</v>
       </c>
       <c r="F17">
-        <f>Norite!H2</f>
+        <f>'Norite Density'!H2</f>
         <v>2.437533180952381E+22</v>
       </c>
       <c r="G17">
@@ -2369,7 +2369,7 @@
         <v>0.98839999999999995</v>
       </c>
       <c r="F18">
-        <f>Norite!H3</f>
+        <f>'Norite Density'!H3</f>
         <v>5.4550738409791042E+20</v>
       </c>
       <c r="G18">
@@ -2403,7 +2403,7 @@
         <v>0.99738000000000004</v>
       </c>
       <c r="F19">
-        <f>Norite!H4</f>
+        <f>'Norite Density'!H4</f>
         <v>4.709608456128509E+23</v>
       </c>
       <c r="G19">
@@ -2437,7 +2437,7 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <f>Norite!H5</f>
+        <f>'Norite Density'!H5</f>
         <v>1.5674854522488044E+22</v>
       </c>
       <c r="G20">
@@ -2471,7 +2471,7 @@
         <v>0.78879999999999995</v>
       </c>
       <c r="F21">
-        <f>Norite!H6</f>
+        <f>'Norite Density'!H6</f>
         <v>2.2240171084468218E+22</v>
       </c>
       <c r="G21">
@@ -2505,7 +2505,7 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <f>Norite!H7</f>
+        <f>'Norite Density'!H7</f>
         <v>5.4637168032021349E+22</v>
       </c>
       <c r="G22">
@@ -2539,7 +2539,7 @@
         <v>0.92191000000000001</v>
       </c>
       <c r="F23">
-        <f>Norite!H8</f>
+        <f>'Norite Density'!H8</f>
         <v>1.5280820436930748E+23</v>
       </c>
       <c r="G23">
@@ -2573,7 +2573,7 @@
         <v>0.93258099999999999</v>
       </c>
       <c r="F24">
-        <f>Norite!H9</f>
+        <f>'Norite Density'!H9</f>
         <v>5.0274355647859225E+21</v>
       </c>
       <c r="G24">
@@ -2607,7 +2607,7 @@
         <v>0.96940999999999999</v>
       </c>
       <c r="F25">
-        <f>Norite!H10</f>
+        <f>'Norite Density'!H10</f>
         <v>2.1252846817505865E+22</v>
       </c>
       <c r="G25">
@@ -2641,7 +2641,7 @@
         <v>0.73719999999999997</v>
       </c>
       <c r="F26">
-        <f>Norite!H13</f>
+        <f>'Norite Density'!H13</f>
         <v>1.7110141617398208E+21</v>
       </c>
       <c r="G26">
@@ -2675,7 +2675,7 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <f>Norite!H11</f>
+        <f>'Norite Density'!H11</f>
         <v>2.9815834169427355E+20</v>
       </c>
       <c r="G27">
@@ -2709,7 +2709,7 @@
         <v>0.91754000000000002</v>
       </c>
       <c r="F28">
-        <f>Norite!H12</f>
+        <f>'Norite Density'!H12</f>
         <v>1.8185581959208526E+22</v>
       </c>
       <c r="G28">

</xml_diff>